<commit_message>
17/10/2024 done with sanity testcases of Campaigns page
</commit_message>
<xml_diff>
--- a/testdata/campaigns_page.xlsx
+++ b/testdata/campaigns_page.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3F74E8-2E33-45B9-B04F-8F93771CE62F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="campaign_details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,45 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Username </t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Result</t>
+    <t>owner</t>
   </si>
   <si>
     <t>abhone@convirza.com</t>
   </si>
-  <si>
-    <t>lmc2demo</t>
-  </si>
-  <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>Invalid</t>
-  </si>
-  <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
-    <t>abc123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abhone@convirza.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">abc@gmail.com </t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,21 +49,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,31 +65,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -402,83 +353,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{376F9C58-89F3-47BA-94CC-97684C5600D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tracking number page is added
</commit_message>
<xml_diff>
--- a/testdata/campaigns_page.xlsx
+++ b/testdata/campaigns_page.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3F74E8-2E33-45B9-B04F-8F93771CE62F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6524ECC3-7C35-4308-9367-CFE6DEB1A26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,7 +357,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>